<commit_message>
update flookup and excel
</commit_message>
<xml_diff>
--- a/test/output_excel.xlsx
+++ b/test/output_excel.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -445,7 +445,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -460,7 +460,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -475,7 +475,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -500,7 +500,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>

</xml_diff>